<commit_message>
Comparaison Masse Frame + AIP
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/Frame_Comparaison.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/Frame_Comparaison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7605AC6-7DCB-45AA-BE80-ABBF497F0FCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9736E27F-E749-4804-BA02-9B5FCDEC3CB7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="252" windowWidth="17280" windowHeight="9060" xr2:uid="{36CB6F9D-CF4D-42B1-A29B-15720D2646A0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{36CB6F9D-CF4D-42B1-A29B-15720D2646A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="25">
   <si>
     <t>Front Bulkhead</t>
   </si>
@@ -69,28 +69,43 @@
     <t>Plancher Cellule Arrière</t>
   </si>
   <si>
-    <t>Triangulations Suspension</t>
-  </si>
-  <si>
-    <t>Invictus</t>
-  </si>
-  <si>
-    <t>Optimus</t>
-  </si>
-  <si>
     <t>Front Hoop Bracing (Forward)</t>
   </si>
   <si>
     <t>Front Hoop Bracing (Rearward)</t>
   </si>
   <si>
-    <t>Tubes Non Structurant Cellule Avant</t>
-  </si>
-  <si>
     <t>Gain (%)</t>
   </si>
   <si>
-    <t>Réduction Masse</t>
+    <t>Tubes Non Structurant Cellule Avant (hors plancher)</t>
+  </si>
+  <si>
+    <t>Triangulations Suspension Arr</t>
+  </si>
+  <si>
+    <t>Triangulation LAS Arr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>Tube Bacquet</t>
+  </si>
+  <si>
+    <t>Comparaison Masse Frame - EPSA</t>
+  </si>
+  <si>
+    <t>Désignation</t>
+  </si>
+  <si>
+    <t>Optimus (kg)</t>
+  </si>
+  <si>
+    <t>Invictus (kg)</t>
+  </si>
+  <si>
+    <t>Réduction Masse (kg)</t>
   </si>
 </sst>
 </file>
@@ -106,15 +121,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -122,17 +149,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -442,256 +520,425 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F88C885E-A80B-484C-9339-F4E74EE96282}">
-  <dimension ref="B5:F21"/>
+  <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="3"/>
+    <col min="2" max="2" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="3"/>
+    <col min="5" max="5" width="16.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D6">
+      <c r="C6" s="4">
+        <f>4*0.38+0.487</f>
+        <v>2.0070000000000001</v>
+      </c>
+      <c r="D6" s="4">
         <f>4*0.359+0.504</f>
         <v>1.94</v>
       </c>
-      <c r="E6">
-        <f>D6-C6</f>
-        <v>1.94</v>
-      </c>
-      <c r="F6" t="e">
-        <f>E6/C6</f>
-        <v>#DIV/0!</v>
+      <c r="E6" s="4">
+        <f>C6-D6</f>
+        <v>6.7000000000000171E-2</v>
+      </c>
+      <c r="F6" s="4">
+        <f>(E6/C6)*100</f>
+        <v>3.3383158943697144</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7">
+      <c r="B7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4">
+        <f>0.721*2</f>
+        <v>1.4419999999999999</v>
+      </c>
+      <c r="D7" s="4">
         <f>0.596*2</f>
         <v>1.1919999999999999</v>
       </c>
-      <c r="E7">
-        <f t="shared" ref="E7:E21" si="0">D7-C7</f>
-        <v>1.1919999999999999</v>
-      </c>
-      <c r="F7" t="e">
-        <f t="shared" ref="F7:F21" si="1">E7/C7</f>
-        <v>#DIV/0!</v>
+      <c r="E7" s="4">
+        <f t="shared" ref="E7:E23" si="0">C7-D7</f>
+        <v>0.25</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" ref="F7:F23" si="1">(E7/C7)*100</f>
+        <v>17.337031900138697</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="4">
         <v>0</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <f>0.31*2</f>
         <v>0.62</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>0.62</v>
-      </c>
-      <c r="F8" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.62</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="C9" s="4">
+        <f>2*(0.296+0.269+0.34+0.331+0.184+0.258+0.319)</f>
+        <v>3.9939999999999998</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>3.9939999999999998</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4">
+        <f>2*(0.166+0.156)+0.306</f>
+        <v>0.95</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4">
+        <f>2*(0.354+0.186+0.113+0.255)+0.319</f>
+        <v>2.1350000000000002</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>2.1350000000000002</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4">
+        <f>0.207+0.208</f>
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4">
+        <f>2*(0.842+0.895+0.811)</f>
+        <v>5.0960000000000001</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0960000000000001</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4">
+        <f>2*0.595</f>
+        <v>1.19</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4">
+        <f t="shared" si="0"/>
+        <v>1.19</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="4">
+        <v>3.569</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>3.569</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="4">
+        <f>2*0.6</f>
+        <v>1.2</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="4">
+        <f>2*(0.175+0.301+0.24+0.457)+0.542</f>
+        <v>2.8879999999999999</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4">
+        <f t="shared" si="0"/>
+        <v>2.8879999999999999</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4">
+        <f t="shared" si="0"/>
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="4">
+        <f>0.092+0.076+0.106+0.019+0.02+0.096+0.075+0.091</f>
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4">
+        <f t="shared" si="0"/>
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="F20" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="4">
+        <f>2*0.285+0.384+0.299+0.3</f>
+        <v>1.5529999999999999</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5529999999999999</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="4">
+        <f>2*(0.075+0.017+0.06+0.08)+0.427</f>
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4">
+        <f t="shared" si="0"/>
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C23" s="4">
+        <f>2*(0.231+0.148+0.121+0.254+0.14+0.211)</f>
+        <v>2.21</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4">
+        <f t="shared" si="0"/>
+        <v>2.21</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="4">
+        <f>SUM(C6:C23)</f>
+        <v>31.228999999999999</v>
+      </c>
+      <c r="D25" s="4">
+        <f>SUM(D6:D23)</f>
+        <v>3.7519999999999998</v>
+      </c>
+      <c r="E25" s="4">
+        <f>C25-D25</f>
+        <v>27.477</v>
+      </c>
+      <c r="F25" s="4">
+        <f>(E25/C25)*100</f>
+        <v>87.985526273655907</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:F3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E6:E23">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Maj Comparaison Frame Invictus-Optimus
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/Frame_Comparaison.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/Frame_Comparaison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9736E27F-E749-4804-BA02-9B5FCDEC3CB7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DABDF6A-4611-4B7C-9CD3-99C96F0E6709}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{36CB6F9D-CF4D-42B1-A29B-15720D2646A0}"/>
+    <workbookView xWindow="312" yWindow="312" windowWidth="17280" windowHeight="9060" xr2:uid="{36CB6F9D-CF4D-42B1-A29B-15720D2646A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Front Bulkhead</t>
   </si>
@@ -176,9 +176,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -191,18 +188,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -523,410 +516,428 @@
   <dimension ref="B1:F25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="11.42578125" style="2"/>
     <col min="2" max="2" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="3"/>
-    <col min="5" max="5" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="3"/>
+    <col min="3" max="4" width="11.42578125" style="2"/>
+    <col min="5" max="5" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <f>4*0.38+0.487</f>
         <v>2.0070000000000001</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <f>4*0.359+0.504</f>
         <v>1.94</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <f>C6-D6</f>
         <v>6.7000000000000171E-2</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <f>(E6/C6)*100</f>
         <v>3.3383158943697144</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <f>0.721*2</f>
         <v>1.4419999999999999</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <f>0.596*2</f>
         <v>1.1919999999999999</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <f t="shared" ref="E7:E23" si="0">C7-D7</f>
         <v>0.25</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <f t="shared" ref="F7:F23" si="1">(E7/C7)*100</f>
         <v>17.337031900138697</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>0</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <f>0.31*2</f>
         <v>0.62</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <f t="shared" si="0"/>
         <v>-0.62</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <f>2*(0.296+0.269+0.34+0.331+0.184+0.258+0.319)</f>
         <v>3.9939999999999998</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4">
-        <f t="shared" si="0"/>
-        <v>3.9939999999999998</v>
-      </c>
-      <c r="F9" s="4">
-        <f t="shared" si="1"/>
-        <v>100</v>
+      <c r="D9" s="3">
+        <f>2*(0.34+0.632+0.123+0.184+0.102+0.19+0.286+0.285)</f>
+        <v>4.2839999999999998</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.29000000000000004</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="1"/>
+        <v>-7.2608913370055097</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <f>2*(0.166+0.156)+0.306</f>
         <v>0.95</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4">
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <f>2*(0.354+0.186+0.113+0.255)+0.319</f>
         <v>2.1350000000000002</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4">
-        <f t="shared" si="0"/>
-        <v>2.1350000000000002</v>
-      </c>
-      <c r="F11" s="4">
-        <f t="shared" si="1"/>
-        <v>100</v>
+      <c r="D11" s="3">
+        <v>1.806</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.32900000000000018</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="1"/>
+        <v>15.409836065573776</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <f>0.207+0.208</f>
         <v>0.41499999999999998</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4">
-        <f t="shared" si="0"/>
-        <v>0.41499999999999998</v>
-      </c>
-      <c r="F12" s="4">
-        <f t="shared" si="1"/>
-        <v>100</v>
+      <c r="D12" s="3">
+        <f>0.236+0.237+2*0.126</f>
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.31</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="1"/>
+        <v>-74.698795180722897</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <f>2*(0.842+0.895+0.811)</f>
         <v>5.0960000000000001</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4">
-        <f t="shared" si="0"/>
-        <v>5.0960000000000001</v>
-      </c>
-      <c r="F13" s="4">
-        <f t="shared" si="1"/>
-        <v>100</v>
+      <c r="D13" s="3">
+        <f>2*(0.792+0.731+0.275+0.615)</f>
+        <v>4.8260000000000005</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.26999999999999957</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="1"/>
+        <v>5.2982731554160045</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <f>2*0.595</f>
         <v>1.19</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4">
-        <f t="shared" si="0"/>
-        <v>1.19</v>
-      </c>
-      <c r="F14" s="4">
+      <c r="D14" s="3">
+        <f>0.575*2</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="1"/>
+        <v>3.3613445378151292</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="F15" s="3">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0.33800000000000002</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4">
-        <f t="shared" si="0"/>
-        <v>0.33800000000000002</v>
-      </c>
-      <c r="F15" s="4">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>3.569</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4">
-        <f t="shared" si="0"/>
-        <v>3.569</v>
-      </c>
-      <c r="F16" s="4">
-        <f t="shared" si="1"/>
-        <v>100</v>
+      <c r="D16" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>6.899999999999995E-2</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="1"/>
+        <v>1.9333146539646948</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <f>2*0.6</f>
         <v>1.2</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <f>2*(0.175+0.301+0.24+0.457)+0.542</f>
         <v>2.8879999999999999</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3">
         <f t="shared" si="0"/>
         <v>2.8879999999999999</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>0.77600000000000002</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4">
+      <c r="D19" s="3"/>
+      <c r="E19" s="3">
         <f t="shared" si="0"/>
         <v>0.77600000000000002</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <f>0.092+0.076+0.106+0.019+0.02+0.096+0.075+0.091</f>
         <v>0.57500000000000007</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3">
         <f t="shared" si="0"/>
         <v>0.57500000000000007</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <f>2*0.285+0.384+0.299+0.3</f>
         <v>1.5529999999999999</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3">
         <f t="shared" si="0"/>
         <v>1.5529999999999999</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <f>2*(0.075+0.017+0.06+0.08)+0.427</f>
         <v>0.89100000000000001</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3">
         <f t="shared" si="0"/>
         <v>0.89100000000000001</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <f>2*(0.231+0.148+0.121+0.254+0.14+0.211)</f>
         <v>2.21</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3">
         <f t="shared" si="0"/>
         <v>2.21</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="3">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <f>SUM(C6:C23)</f>
         <v>31.228999999999999</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <f>SUM(D6:D23)</f>
-        <v>3.7519999999999998</v>
-      </c>
-      <c r="E25" s="4">
+        <v>20.042999999999999</v>
+      </c>
+      <c r="E25" s="3">
         <f>C25-D25</f>
-        <v>27.477</v>
-      </c>
-      <c r="F25" s="4">
+        <v>11.186</v>
+      </c>
+      <c r="F25" s="3">
         <f>(E25/C25)*100</f>
-        <v>87.985526273655907</v>
+        <v>35.819270549809474</v>
       </c>
     </row>
   </sheetData>
@@ -934,7 +945,7 @@
     <mergeCell ref="C1:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="E6:E23">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
MAJ Cas de charge Frame + Placement Sleeved Joint
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/Frame_Comparaison.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/Frame_Comparaison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DABDF6A-4611-4B7C-9CD3-99C96F0E6709}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B57D3E-6933-49A7-90B5-07C195EA0C83}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="312" yWindow="312" windowWidth="17280" windowHeight="9060" xr2:uid="{36CB6F9D-CF4D-42B1-A29B-15720D2646A0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{36CB6F9D-CF4D-42B1-A29B-15720D2646A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Front Bulkhead</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Réduction Masse (kg)</t>
+  </si>
+  <si>
+    <t>Sleeved Joint / Lug Joint</t>
   </si>
 </sst>
 </file>
@@ -168,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -187,6 +190,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -513,43 +519,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F88C885E-A80B-484C-9339-F4E74EE96282}">
-  <dimension ref="B1:F25"/>
+  <dimension ref="B1:F26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2"/>
-    <col min="2" max="2" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="2"/>
-    <col min="5" max="5" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="11.44140625" style="2"/>
+    <col min="2" max="2" width="33.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.44140625" style="2"/>
+    <col min="5" max="5" width="16.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="5" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
@@ -566,7 +572,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -587,7 +593,7 @@
         <v>3.3383158943697144</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
@@ -600,15 +606,15 @@
         <v>1.1919999999999999</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" ref="E7:E23" si="0">C7-D7</f>
+        <f t="shared" ref="E7:E24" si="0">C7-D7</f>
         <v>0.25</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ref="F7:F23" si="1">(E7/C7)*100</f>
+        <f t="shared" ref="F7:F24" si="1">(E7/C7)*100</f>
         <v>17.337031900138697</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
@@ -627,7 +633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
@@ -648,7 +654,7 @@
         <v>-7.2608913370055097</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
@@ -668,7 +674,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>3</v>
       </c>
@@ -688,7 +694,7 @@
         <v>15.409836065573776</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
@@ -709,7 +715,7 @@
         <v>-74.698795180722897</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>2</v>
       </c>
@@ -730,7 +736,7 @@
         <v>5.2982731554160045</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>5</v>
       </c>
@@ -751,7 +757,7 @@
         <v>3.3613445378151292</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
@@ -768,7 +774,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
@@ -787,7 +793,7 @@
         <v>1.9333146539646948</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>7</v>
       </c>
@@ -805,7 +811,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>8</v>
       </c>
@@ -823,7 +829,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>9</v>
       </c>
@@ -840,7 +846,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
@@ -858,7 +864,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>11</v>
       </c>
@@ -876,7 +882,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>16</v>
       </c>
@@ -894,7 +900,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
         <v>17</v>
       </c>
@@ -912,39 +918,60 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
+    <row r="24" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="3">
+        <f>2*0.155</f>
+        <v>0.31</v>
+      </c>
+      <c r="D24" s="3">
+        <f>2*0.107</f>
+        <v>0.214</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="1"/>
+        <v>30.967741935483872</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="6"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="3">
-        <f>SUM(C6:C23)</f>
-        <v>31.228999999999999</v>
-      </c>
-      <c r="D25" s="3">
-        <f>SUM(D6:D23)</f>
-        <v>20.042999999999999</v>
-      </c>
-      <c r="E25" s="3">
-        <f>C25-D25</f>
-        <v>11.186</v>
-      </c>
-      <c r="F25" s="3">
-        <f>(E25/C25)*100</f>
-        <v>35.819270549809474</v>
+      <c r="C26" s="3">
+        <f>SUM(C6:C24)</f>
+        <v>31.538999999999998</v>
+      </c>
+      <c r="D26" s="3">
+        <f>SUM(D6:D24)</f>
+        <v>20.256999999999998</v>
+      </c>
+      <c r="E26" s="3">
+        <f>C26-D26</f>
+        <v>11.282</v>
+      </c>
+      <c r="F26" s="3">
+        <f>(E26/C26)*100</f>
+        <v>35.77158438758363</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F3"/>
   </mergeCells>
-  <conditionalFormatting sqref="E6:E23">
+  <conditionalFormatting sqref="E6:E24">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
MAJ Masse Frame Invictus
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/Frame_Comparaison.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/Frame_Comparaison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31E880F-2151-4467-BEA2-0ED1E8692916}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5410054-87EE-48E0-8AE9-E81A5EAFF5AF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{36CB6F9D-CF4D-42B1-A29B-15720D2646A0}"/>
   </bookViews>
@@ -180,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -206,24 +206,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -551,7 +550,7 @@
   <dimension ref="B1:F27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,24 +564,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="5" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
@@ -617,7 +616,7 @@
         <f>C6-D6</f>
         <v>6.7000000000000171E-2</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="11">
         <f>(E6/C6)*100</f>
         <v>3.3383158943697144</v>
       </c>
@@ -638,7 +637,7 @@
         <f t="shared" ref="E7:E25" si="0">C7-D7</f>
         <v>0.25</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="11">
         <f t="shared" ref="F7:F25" si="1">(E7/C7)*100</f>
         <v>17.337031900138697</v>
       </c>
@@ -658,7 +657,7 @@
         <f t="shared" si="0"/>
         <v>-0.62</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="11">
         <v>0</v>
       </c>
     </row>
@@ -678,12 +677,12 @@
         <f t="shared" si="0"/>
         <v>-0.35600000000000076</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="11">
         <f t="shared" si="1"/>
         <v>-8.9133700550826429</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
@@ -698,7 +697,7 @@
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="11">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -718,7 +717,7 @@
         <f t="shared" si="0"/>
         <v>0.10200000000000031</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="11">
         <f t="shared" si="1"/>
         <v>4.7775175644028245</v>
       </c>
@@ -739,7 +738,7 @@
         <f t="shared" si="0"/>
         <v>-0.31</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="11">
         <f t="shared" si="1"/>
         <v>-74.698795180722897</v>
       </c>
@@ -760,7 +759,7 @@
         <f t="shared" si="0"/>
         <v>0.26999999999999957</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="11">
         <f t="shared" si="1"/>
         <v>5.2982731554160045</v>
       </c>
@@ -781,7 +780,7 @@
         <f t="shared" si="0"/>
         <v>4.0000000000000036E-2</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="11">
         <f t="shared" si="1"/>
         <v>3.3613445378151292</v>
       </c>
@@ -800,7 +799,7 @@
         <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="11">
         <f t="shared" si="1"/>
         <v>50.295857988165679</v>
       </c>
@@ -819,7 +818,7 @@
         <f t="shared" si="0"/>
         <v>0.12800000000000011</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="11">
         <f t="shared" si="1"/>
         <v>3.5864387783692941</v>
       </c>
@@ -840,7 +839,7 @@
         <f t="shared" si="0"/>
         <v>-0.35600000000000009</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="11">
         <f t="shared" si="1"/>
         <v>-29.666666666666675</v>
       </c>
@@ -861,7 +860,7 @@
         <f t="shared" si="0"/>
         <v>-0.87400000000000011</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="11">
         <f t="shared" si="1"/>
         <v>-30.263157894736846</v>
       </c>
@@ -880,7 +879,7 @@
         <f t="shared" si="0"/>
         <v>5.4000000000000048E-2</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="11">
         <f t="shared" si="1"/>
         <v>6.9587628865979436</v>
       </c>
@@ -901,7 +900,7 @@
         <f t="shared" si="0"/>
         <v>0.16400000000000003</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="11">
         <f t="shared" si="1"/>
         <v>28.521739130434788</v>
       </c>
@@ -922,7 +921,7 @@
         <f t="shared" si="0"/>
         <v>-0.35699999999999998</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="11">
         <f t="shared" si="1"/>
         <v>-22.98776561493883</v>
       </c>
@@ -943,7 +942,7 @@
         <f t="shared" si="0"/>
         <v>-0.19099999999999984</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="11">
         <f t="shared" si="1"/>
         <v>-21.436588103254749</v>
       </c>
@@ -964,7 +963,7 @@
         <f t="shared" si="0"/>
         <v>1.8079999999999998</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="11">
         <f t="shared" si="1"/>
         <v>81.809954751131215</v>
       </c>
@@ -985,7 +984,7 @@
         <f t="shared" si="0"/>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="11">
         <f t="shared" si="1"/>
         <v>30.967741935483872</v>
       </c>
@@ -1006,7 +1005,7 @@
         <f t="shared" si="0"/>
         <v>0.12400000000000005</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="11">
         <f t="shared" si="1"/>
         <v>28.83720930232559</v>
       </c>
@@ -1016,25 +1015,25 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="9">
         <f>SUM(C6:C25)</f>
         <v>31.968999999999998</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="9">
         <f>SUM(D6:D25)</f>
         <v>30.810000000000002</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="9">
         <f>C27-D27</f>
         <v>1.1589999999999954</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="12">
         <f>(E27/C27)*100</f>
         <v>3.6253870937470531</v>
       </c>
@@ -1044,10 +1043,10 @@
     <mergeCell ref="C1:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="E6:E25">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Avancée Diapo Rencontre Gir
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/Frame_Comparaison.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/Frame_Comparaison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5410054-87EE-48E0-8AE9-E81A5EAFF5AF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46C9FB9-9C13-4085-9575-1538156A22F6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{36CB6F9D-CF4D-42B1-A29B-15720D2646A0}"/>
   </bookViews>
@@ -209,13 +209,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -550,7 +550,7 @@
   <dimension ref="B1:F27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,24 +564,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="5" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
@@ -609,16 +609,16 @@
         <v>2.0070000000000001</v>
       </c>
       <c r="D6" s="3">
-        <f>4*0.359+0.504</f>
-        <v>1.94</v>
+        <f>2*0.353+2*0.359+0.46</f>
+        <v>1.8839999999999999</v>
       </c>
       <c r="E6" s="3">
         <f>C6-D6</f>
-        <v>6.7000000000000171E-2</v>
-      </c>
-      <c r="F6" s="11">
+        <v>0.12300000000000022</v>
+      </c>
+      <c r="F6" s="10">
         <f>(E6/C6)*100</f>
-        <v>3.3383158943697144</v>
+        <v>6.1285500747384258</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -630,16 +630,16 @@
         <v>1.4419999999999999</v>
       </c>
       <c r="D7" s="3">
-        <f>0.596*2</f>
-        <v>1.1919999999999999</v>
+        <f>0.646*2</f>
+        <v>1.292</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" ref="E7:E25" si="0">C7-D7</f>
-        <v>0.25</v>
-      </c>
-      <c r="F7" s="11">
+        <v>0.14999999999999991</v>
+      </c>
+      <c r="F7" s="10">
         <f t="shared" ref="F7:F25" si="1">(E7/C7)*100</f>
-        <v>17.337031900138697</v>
+        <v>10.402219140083211</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -650,14 +650,14 @@
         <v>0</v>
       </c>
       <c r="D8" s="3">
-        <f>0.31*2</f>
-        <v>0.62</v>
+        <f>0.404*2</f>
+        <v>0.80800000000000005</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>-0.62</v>
-      </c>
-      <c r="F8" s="11">
+        <v>-0.80800000000000005</v>
+      </c>
+      <c r="F8" s="10">
         <v>0</v>
       </c>
     </row>
@@ -670,16 +670,16 @@
         <v>3.9939999999999998</v>
       </c>
       <c r="D9" s="3">
-        <f>2*(0.34+0.632+0.123+0.184+0.102+0.223+0.286+0.285)</f>
-        <v>4.3500000000000005</v>
+        <f>2*(0.37+0.379+0.194+0.32+0.274+0.116+0.112+0.272)</f>
+        <v>4.0740000000000007</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>-0.35600000000000076</v>
-      </c>
-      <c r="F9" s="11">
-        <f t="shared" si="1"/>
-        <v>-8.9133700550826429</v>
+        <v>-8.0000000000000959E-2</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" si="1"/>
+        <v>-2.0030045067601643</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
@@ -697,7 +697,7 @@
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
@@ -711,15 +711,15 @@
         <v>2.1350000000000002</v>
       </c>
       <c r="D11" s="3">
-        <v>2.0329999999999999</v>
+        <v>2.0470000000000002</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="0"/>
-        <v>0.10200000000000031</v>
-      </c>
-      <c r="F11" s="11">
-        <f t="shared" si="1"/>
-        <v>4.7775175644028245</v>
+        <v>8.8000000000000078E-2</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" si="1"/>
+        <v>4.1217798594847812</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
@@ -731,16 +731,16 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="D12" s="3">
-        <f>0.236+0.237+2*0.126</f>
-        <v>0.72499999999999998</v>
+        <f>0.22+0.218+0.116+0.057+0.056</f>
+        <v>0.66700000000000015</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>-0.31</v>
-      </c>
-      <c r="F12" s="11">
-        <f t="shared" si="1"/>
-        <v>-74.698795180722897</v>
+        <v>-0.25200000000000017</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="1"/>
+        <v>-60.722891566265105</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
@@ -752,16 +752,16 @@
         <v>5.0960000000000001</v>
       </c>
       <c r="D13" s="3">
-        <f>2*(0.792+0.731+0.275+0.615)</f>
-        <v>4.8260000000000005</v>
+        <f>2*(0.768+0.708+0.258+0.546+0.404)</f>
+        <v>5.3680000000000003</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="0"/>
-        <v>0.26999999999999957</v>
-      </c>
-      <c r="F13" s="11">
-        <f t="shared" si="1"/>
-        <v>5.2982731554160045</v>
+        <v>-0.27200000000000024</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" si="1"/>
+        <v>-5.3375196232339137</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
@@ -773,16 +773,16 @@
         <v>1.19</v>
       </c>
       <c r="D14" s="3">
-        <f>0.575*2</f>
-        <v>1.1499999999999999</v>
+        <f>0.537+0.233+0.292</f>
+        <v>1.0620000000000001</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="0"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F14" s="11">
-        <f t="shared" si="1"/>
-        <v>3.3613445378151292</v>
+        <v>0.12799999999999989</v>
+      </c>
+      <c r="F14" s="10">
+        <f t="shared" si="1"/>
+        <v>10.756302521008394</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
@@ -793,15 +793,15 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D15" s="3">
-        <v>0.16800000000000001</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" si="0"/>
-        <v>0.17</v>
-      </c>
-      <c r="F15" s="11">
-        <f t="shared" si="1"/>
-        <v>50.295857988165679</v>
+        <v>0.17600000000000002</v>
+      </c>
+      <c r="F15" s="10">
+        <f t="shared" si="1"/>
+        <v>52.071005917159766</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
@@ -812,15 +812,15 @@
         <v>3.569</v>
       </c>
       <c r="D16" s="3">
-        <v>3.4409999999999998</v>
+        <v>3.573</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="0"/>
-        <v>0.12800000000000011</v>
-      </c>
-      <c r="F16" s="11">
-        <f t="shared" si="1"/>
-        <v>3.5864387783692941</v>
+        <v>-4.0000000000000036E-3</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" si="1"/>
+        <v>-0.11207621182404044</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
@@ -832,16 +832,16 @@
         <v>1.2</v>
       </c>
       <c r="D17" s="3">
-        <f>2*0.778</f>
-        <v>1.556</v>
+        <f>2*0.779</f>
+        <v>1.5580000000000001</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="0"/>
-        <v>-0.35600000000000009</v>
-      </c>
-      <c r="F17" s="11">
-        <f t="shared" si="1"/>
-        <v>-29.666666666666675</v>
+        <v>-0.3580000000000001</v>
+      </c>
+      <c r="F17" s="10">
+        <f t="shared" si="1"/>
+        <v>-29.833333333333346</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
@@ -853,16 +853,16 @@
         <v>2.8879999999999999</v>
       </c>
       <c r="D18" s="3">
-        <f>2*(0.232+0.319+0.212+0.407+0.488)+0.446</f>
-        <v>3.762</v>
+        <f>2*(0.22+0.222+0.289+0.37+0.199+0.478)+0.446</f>
+        <v>4.0019999999999998</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="0"/>
-        <v>-0.87400000000000011</v>
-      </c>
-      <c r="F18" s="11">
-        <f t="shared" si="1"/>
-        <v>-30.263157894736846</v>
+        <v>-1.1139999999999999</v>
+      </c>
+      <c r="F18" s="10">
+        <f t="shared" si="1"/>
+        <v>-38.573407202216067</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
@@ -873,15 +873,15 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="D19" s="3">
-        <v>0.72199999999999998</v>
+        <v>0.70699999999999996</v>
       </c>
       <c r="E19" s="3">
         <f t="shared" si="0"/>
-        <v>5.4000000000000048E-2</v>
-      </c>
-      <c r="F19" s="11">
-        <f t="shared" si="1"/>
-        <v>6.9587628865979436</v>
+        <v>6.9000000000000061E-2</v>
+      </c>
+      <c r="F19" s="10">
+        <f t="shared" si="1"/>
+        <v>8.8917525773195951</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
@@ -900,7 +900,7 @@
         <f t="shared" si="0"/>
         <v>0.16400000000000003</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="10">
         <f t="shared" si="1"/>
         <v>28.521739130434788</v>
       </c>
@@ -921,7 +921,7 @@
         <f t="shared" si="0"/>
         <v>-0.35699999999999998</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="10">
         <f t="shared" si="1"/>
         <v>-22.98776561493883</v>
       </c>
@@ -942,7 +942,7 @@
         <f t="shared" si="0"/>
         <v>-0.19099999999999984</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="10">
         <f t="shared" si="1"/>
         <v>-21.436588103254749</v>
       </c>
@@ -963,7 +963,7 @@
         <f t="shared" si="0"/>
         <v>1.8079999999999998</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="10">
         <f t="shared" si="1"/>
         <v>81.809954751131215</v>
       </c>
@@ -984,7 +984,7 @@
         <f t="shared" si="0"/>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="10">
         <f t="shared" si="1"/>
         <v>30.967741935483872</v>
       </c>
@@ -1005,7 +1005,7 @@
         <f t="shared" si="0"/>
         <v>0.12400000000000005</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="10">
         <f t="shared" si="1"/>
         <v>28.83720930232559</v>
       </c>
@@ -1015,7 +1015,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="11"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
@@ -1027,15 +1027,15 @@
       </c>
       <c r="D27" s="9">
         <f>SUM(D6:D25)</f>
-        <v>30.810000000000002</v>
+        <v>31.529000000000003</v>
       </c>
       <c r="E27" s="9">
         <f>C27-D27</f>
-        <v>1.1589999999999954</v>
-      </c>
-      <c r="F27" s="12">
+        <v>0.43999999999999417</v>
+      </c>
+      <c r="F27" s="11">
         <f>(E27/C27)*100</f>
-        <v>3.6253870937470531</v>
+        <v>1.3763333229065475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MAJ Formation Frame - Again
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/Frame_Comparaison.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/Frame_Comparaison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6867B68E-865D-485E-BC79-628A75663130}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1DF1B7-10A8-4148-B2C2-13661F442D5B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{36CB6F9D-CF4D-42B1-A29B-15720D2646A0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Front Bulkhead</t>
   </si>
@@ -112,14 +112,36 @@
   </si>
   <si>
     <t>Triangulation Transmission secondaire</t>
+  </si>
+  <si>
+    <t>Invictus si min règlement sections</t>
+  </si>
+  <si>
+    <t>MAJ : CMI - 09/04/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -180,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -217,6 +239,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F88C885E-A80B-484C-9339-F4E74EE96282}">
-  <dimension ref="B1:F27"/>
+  <dimension ref="B1:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,27 +591,27 @@
     <col min="7" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C1" s="12" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="5" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="5" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
@@ -599,8 +627,17 @@
       <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -620,8 +657,20 @@
         <f>(E6/C6)*100</f>
         <v>6.1285500747384258</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J6" s="3">
+        <f>2*0.353+2*0.359+0.46</f>
+        <v>1.8839999999999999</v>
+      </c>
+      <c r="K6" s="3">
+        <f>J6*0.95</f>
+        <v>1.7897999999999998</v>
+      </c>
+      <c r="L6" s="3">
+        <f>100*(J6-K6)/J6</f>
+        <v>5.0000000000000027</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
@@ -641,8 +690,20 @@
         <f t="shared" ref="F7:F25" si="1">(E7/C7)*100</f>
         <v>10.402219140083211</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J7" s="3">
+        <f>0.646*2</f>
+        <v>1.292</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" ref="K7:K8" si="2">J7*0.95</f>
+        <v>1.2274</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" ref="L7:L27" si="3">100*(J7-K7)/J7</f>
+        <v>4.9999999999999991</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
@@ -660,8 +721,20 @@
       <c r="F8" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J8" s="3">
+        <f>0.404*2</f>
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.76760000000000006</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="3"/>
+        <v>4.9999999999999982</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
@@ -681,8 +754,20 @@
         <f t="shared" si="1"/>
         <v>-2.0030045067601643</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J9" s="3">
+        <f>2*(0.37+0.379+0.194+0.32+0.274+0.116+0.112+0.272)</f>
+        <v>4.0740000000000007</v>
+      </c>
+      <c r="K9" s="3">
+        <f>J9*0.8</f>
+        <v>3.2592000000000008</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="3"/>
+        <v>19.999999999999993</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
@@ -701,8 +786,17 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>3</v>
       </c>
@@ -721,8 +815,18 @@
         <f t="shared" si="1"/>
         <v>4.1217798594847812</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J11" s="3">
+        <v>2.0470000000000002</v>
+      </c>
+      <c r="K11" s="3">
+        <v>2.0470000000000002</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
@@ -742,8 +846,18 @@
         <f t="shared" si="1"/>
         <v>-60.722891566265105</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J12" s="3">
+        <f>0.22+0.218+0.116+0.057+0.056</f>
+        <v>0.66700000000000015</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>2</v>
       </c>
@@ -763,8 +877,20 @@
         <f t="shared" si="1"/>
         <v>-5.3375196232339137</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J13" s="3">
+        <f>2*(0.768+0.708+0.258+0.546+0.404)</f>
+        <v>5.3680000000000003</v>
+      </c>
+      <c r="K13" s="3">
+        <f>J13*0.95</f>
+        <v>5.0995999999999997</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" si="3"/>
+        <v>5.0000000000000115</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>5</v>
       </c>
@@ -784,8 +910,19 @@
         <f t="shared" si="1"/>
         <v>10.756302521008394</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J14" s="3">
+        <f>0.537+0.233+0.292</f>
+        <v>1.0620000000000001</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1.0620000000000001</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
@@ -803,8 +940,18 @@
         <f t="shared" si="1"/>
         <v>52.071005917159766</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J15" s="3">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
@@ -822,8 +969,18 @@
         <f t="shared" si="1"/>
         <v>-0.11207621182404044</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J16" s="3">
+        <v>3.573</v>
+      </c>
+      <c r="K16" s="3">
+        <v>3.573</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>7</v>
       </c>
@@ -843,8 +1000,20 @@
         <f t="shared" si="1"/>
         <v>-30.166666666666675</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J17" s="3">
+        <f>2*0.781</f>
+        <v>1.5620000000000001</v>
+      </c>
+      <c r="K17" s="3">
+        <f>J17*0.95</f>
+        <v>1.4839</v>
+      </c>
+      <c r="L17" s="3">
+        <f t="shared" si="3"/>
+        <v>5.0000000000000036</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>8</v>
       </c>
@@ -864,8 +1033,20 @@
         <f t="shared" si="1"/>
         <v>-38.573407202216067</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J18" s="3">
+        <f>2*(0.22+0.222+0.289+0.37+0.199+0.478)+0.446</f>
+        <v>4.0019999999999998</v>
+      </c>
+      <c r="K18" s="3">
+        <f>J18*0.8</f>
+        <v>3.2016</v>
+      </c>
+      <c r="L18" s="3">
+        <f t="shared" si="3"/>
+        <v>19.999999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>9</v>
       </c>
@@ -883,8 +1064,18 @@
         <f t="shared" si="1"/>
         <v>8.8917525773195951</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J19" s="3">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
@@ -904,8 +1095,18 @@
         <f t="shared" si="1"/>
         <v>28.521739130434788</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J20" s="3">
+        <f>0.066+0.054+0.069+4*0.008+0.067+0.068+0.055</f>
+        <v>0.41100000000000003</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>11</v>
       </c>
@@ -925,8 +1126,18 @@
         <f t="shared" si="1"/>
         <v>-35.028976175144855</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J21" s="3">
+        <f>0.274+0.247+0.19+0.206+0.117+0.053+0.061+2*(0.139+0.228)+0.109+0.052+0.054</f>
+        <v>2.0969999999999995</v>
+      </c>
+      <c r="K21" s="3">
+        <v>2.097</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>16</v>
       </c>
@@ -946,8 +1157,19 @@
         <f t="shared" si="1"/>
         <v>-15.375982042648712</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J22" s="3">
+        <f>2*(0.079+0.158+0.147)+0.26</f>
+        <v>1.028</v>
+      </c>
+      <c r="K22" s="3">
+        <v>1.028</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
         <v>17</v>
       </c>
@@ -967,8 +1189,19 @@
         <f t="shared" si="1"/>
         <v>65.067873303167417</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="3">
+        <f>2*(0.106+0.103)+0.354</f>
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
         <v>25</v>
       </c>
@@ -988,8 +1221,19 @@
         <f t="shared" si="1"/>
         <v>30.967741935483872</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="J24" s="3">
+        <f>2*0.107</f>
+        <v>0.214</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0.214</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
         <v>26</v>
       </c>
@@ -1009,15 +1253,27 @@
         <f t="shared" si="1"/>
         <v>36.97674418604651</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J25" s="3">
+        <f>0.086+2*(0.054)+0.022+0.055</f>
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="L25" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="L26" s="12"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
         <v>18</v>
       </c>
@@ -1036,6 +1292,23 @@
       <c r="F27" s="11">
         <f>(E27/C27)*100</f>
         <v>-0.10009696893865942</v>
+      </c>
+      <c r="J27" s="9">
+        <f>SUM(J6:J25)</f>
+        <v>32.000999999999998</v>
+      </c>
+      <c r="K27" s="9">
+        <f>SUM(K6:K25)</f>
+        <v>29.8401</v>
+      </c>
+      <c r="L27" s="3">
+        <f t="shared" si="3"/>
+        <v>6.7526014812037065</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B31" s="14" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>